<commit_message>
Fix: update cash_parser and import into asset_value
</commit_message>
<xml_diff>
--- a/data/cash_accounts.xlsx
+++ b/data/cash_accounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanchuang/Desktop/資產計算/investment_tracker/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138D4E21-0CE5-4345-94C2-899A60FBBC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A12235-1AD7-E14D-BD85-AA9DEA8EB75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="monthly_balance" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">monthly_balance!$A$1:$I$319</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">monthly_balance!$A$1:$I$325</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1654" uniqueCount="37">
   <si>
     <t>Sean</t>
   </si>
@@ -190,18 +190,6 @@
         <charset val="136"/>
       </rPr>
       <t>外幣帳戶</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>定存</t>
     </r>
   </si>
   <si>
@@ -494,6 +482,22 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>美金定存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>First Trade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>投資帳戶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -502,7 +506,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,6 +553,13 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+      <charset val="136"/>
     </font>
     <font>
       <sz val="12"/>
@@ -599,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -620,6 +631,8 @@
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -924,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I325"/>
+  <dimension ref="A1:I327"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A300" zoomScale="133" workbookViewId="0">
-      <selection activeCell="D330" sqref="D330"/>
+      <selection activeCell="E328" sqref="E328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -960,13 +973,13 @@
         <v>8</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>9</v>
@@ -1320,8 +1333,8 @@
       <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>17</v>
+      <c r="D15" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>1</v>
@@ -1388,7 +1401,7 @@
         <v>80</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1427,8 +1440,8 @@
       <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>17</v>
+      <c r="D19" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>0</v>
@@ -1453,8 +1466,8 @@
       <c r="C20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>17</v>
+      <c r="D20" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>1</v>
@@ -1557,8 +1570,8 @@
       <c r="C24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>17</v>
+      <c r="D24" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>0</v>
@@ -1583,8 +1596,8 @@
       <c r="C25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>17</v>
+      <c r="D25" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>1</v>
@@ -1687,8 +1700,8 @@
       <c r="C29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>17</v>
+      <c r="D29" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>0</v>
@@ -1713,8 +1726,8 @@
       <c r="C30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>17</v>
+      <c r="D30" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>1</v>
@@ -1755,7 +1768,7 @@
         <v>558401</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1820,8 +1833,8 @@
       <c r="C34" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>17</v>
+      <c r="D34" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>0</v>
@@ -1846,8 +1859,8 @@
       <c r="C35" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>17</v>
+      <c r="D35" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>1</v>
@@ -1950,8 +1963,8 @@
       <c r="C39" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>17</v>
+      <c r="D39" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>0</v>
@@ -1976,8 +1989,8 @@
       <c r="C40" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>17</v>
+      <c r="D40" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>1</v>
@@ -2080,8 +2093,8 @@
       <c r="C44" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>17</v>
+      <c r="D44" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>0</v>
@@ -2106,8 +2119,8 @@
       <c r="C45" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>17</v>
+      <c r="D45" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>1</v>
@@ -2210,8 +2223,8 @@
       <c r="C49" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>17</v>
+      <c r="D49" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>0</v>
@@ -2236,8 +2249,8 @@
       <c r="C50" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>17</v>
+      <c r="D50" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>1</v>
@@ -2278,7 +2291,7 @@
         <v>926522</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2343,8 +2356,8 @@
       <c r="C54" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>17</v>
+      <c r="D54" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>0</v>
@@ -2369,8 +2382,8 @@
       <c r="C55" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>17</v>
+      <c r="D55" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>1</v>
@@ -2437,7 +2450,7 @@
         <v>649442</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2476,8 +2489,8 @@
       <c r="C59" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>17</v>
+      <c r="D59" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>0</v>
@@ -2502,8 +2515,8 @@
       <c r="C60" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>17</v>
+      <c r="D60" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>1</v>
@@ -2570,7 +2583,7 @@
         <v>649442</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2609,8 +2622,8 @@
       <c r="C64" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>17</v>
+      <c r="D64" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>0</v>
@@ -2635,8 +2648,8 @@
       <c r="C65" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>17</v>
+      <c r="D65" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>1</v>
@@ -2739,8 +2752,8 @@
       <c r="C69" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>17</v>
+      <c r="D69" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>0</v>
@@ -2765,8 +2778,8 @@
       <c r="C70" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>17</v>
+      <c r="D70" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>1</v>
@@ -2869,8 +2882,8 @@
       <c r="C74" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>17</v>
+      <c r="D74" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>0</v>
@@ -2895,8 +2908,8 @@
       <c r="C75" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>17</v>
+      <c r="D75" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>1</v>
@@ -2999,8 +3012,8 @@
       <c r="C79" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>17</v>
+      <c r="D79" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>0</v>
@@ -3025,8 +3038,8 @@
       <c r="C80" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>17</v>
+      <c r="D80" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>1</v>
@@ -3093,7 +3106,7 @@
         <v>884</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3132,8 +3145,8 @@
       <c r="C84" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>17</v>
+      <c r="D84" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>0</v>
@@ -3158,8 +3171,8 @@
       <c r="C85" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>17</v>
+      <c r="D85" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>1</v>
@@ -3200,7 +3213,7 @@
         <v>82564</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3265,8 +3278,8 @@
       <c r="C89" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D89" s="2" t="s">
-        <v>17</v>
+      <c r="D89" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>0</v>
@@ -3291,8 +3304,8 @@
       <c r="C90" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>17</v>
+      <c r="D90" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>1</v>
@@ -3395,8 +3408,8 @@
       <c r="C94" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>17</v>
+      <c r="D94" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>0</v>
@@ -3421,8 +3434,8 @@
       <c r="C95" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D95" s="2" t="s">
-        <v>17</v>
+      <c r="D95" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>1</v>
@@ -3525,8 +3538,8 @@
       <c r="C99" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>17</v>
+      <c r="D99" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>0</v>
@@ -3551,8 +3564,8 @@
       <c r="C100" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D100" s="2" t="s">
-        <v>17</v>
+      <c r="D100" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>1</v>
@@ -3655,8 +3668,8 @@
       <c r="C104" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D104" s="2" t="s">
-        <v>17</v>
+      <c r="D104" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E104" s="5" t="s">
         <v>0</v>
@@ -3681,8 +3694,8 @@
       <c r="C105" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D105" s="2" t="s">
-        <v>17</v>
+      <c r="D105" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E105" s="5" t="s">
         <v>1</v>
@@ -3785,8 +3798,8 @@
       <c r="C109" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D109" s="2" t="s">
-        <v>17</v>
+      <c r="D109" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E109" s="5" t="s">
         <v>0</v>
@@ -3811,8 +3824,8 @@
       <c r="C110" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D110" s="2" t="s">
-        <v>17</v>
+      <c r="D110" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E110" s="5" t="s">
         <v>1</v>
@@ -3915,8 +3928,8 @@
       <c r="C114" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D114" s="2" t="s">
-        <v>17</v>
+      <c r="D114" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E114" s="5" t="s">
         <v>0</v>
@@ -3941,8 +3954,8 @@
       <c r="C115" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D115" s="2" t="s">
-        <v>17</v>
+      <c r="D115" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E115" s="5" t="s">
         <v>1</v>
@@ -4045,8 +4058,8 @@
       <c r="C119" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D119" s="2" t="s">
-        <v>17</v>
+      <c r="D119" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>0</v>
@@ -4071,8 +4084,8 @@
       <c r="C120" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D120" s="2" t="s">
-        <v>17</v>
+      <c r="D120" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E120" s="5" t="s">
         <v>1</v>
@@ -4175,8 +4188,8 @@
       <c r="C124" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D124" s="2" t="s">
-        <v>17</v>
+      <c r="D124" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E124" s="5" t="s">
         <v>0</v>
@@ -4201,8 +4214,8 @@
       <c r="C125" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D125" s="2" t="s">
-        <v>17</v>
+      <c r="D125" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E125" s="5" t="s">
         <v>1</v>
@@ -4243,7 +4256,7 @@
         <v>40951</v>
       </c>
       <c r="I126" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -4308,8 +4321,8 @@
       <c r="C129" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D129" s="2" t="s">
-        <v>17</v>
+      <c r="D129" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E129" s="5" t="s">
         <v>0</v>
@@ -4334,8 +4347,8 @@
       <c r="C130" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D130" s="2" t="s">
-        <v>17</v>
+      <c r="D130" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E130" s="5" t="s">
         <v>1</v>
@@ -4438,8 +4451,8 @@
       <c r="C134" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D134" s="2" t="s">
-        <v>17</v>
+      <c r="D134" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E134" s="5" t="s">
         <v>0</v>
@@ -4464,8 +4477,8 @@
       <c r="C135" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D135" s="2" t="s">
-        <v>17</v>
+      <c r="D135" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E135" s="5" t="s">
         <v>1</v>
@@ -4568,8 +4581,8 @@
       <c r="C139" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D139" s="2" t="s">
-        <v>17</v>
+      <c r="D139" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E139" s="5" t="s">
         <v>0</v>
@@ -4594,8 +4607,8 @@
       <c r="C140" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D140" s="2" t="s">
-        <v>17</v>
+      <c r="D140" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E140" s="5" t="s">
         <v>1</v>
@@ -4698,8 +4711,8 @@
       <c r="C144" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D144" s="2" t="s">
-        <v>17</v>
+      <c r="D144" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E144" s="5" t="s">
         <v>0</v>
@@ -4724,8 +4737,8 @@
       <c r="C145" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D145" s="2" t="s">
-        <v>17</v>
+      <c r="D145" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E145" s="5" t="s">
         <v>1</v>
@@ -4828,8 +4841,8 @@
       <c r="C149" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D149" s="2" t="s">
-        <v>17</v>
+      <c r="D149" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E149" s="5" t="s">
         <v>0</v>
@@ -4854,8 +4867,8 @@
       <c r="C150" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D150" s="2" t="s">
-        <v>17</v>
+      <c r="D150" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E150" s="5" t="s">
         <v>1</v>
@@ -4958,8 +4971,8 @@
       <c r="C154" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D154" s="2" t="s">
-        <v>17</v>
+      <c r="D154" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E154" s="5" t="s">
         <v>0</v>
@@ -4984,8 +4997,8 @@
       <c r="C155" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D155" s="2" t="s">
-        <v>17</v>
+      <c r="D155" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E155" s="5" t="s">
         <v>1</v>
@@ -5088,8 +5101,8 @@
       <c r="C159" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D159" s="2" t="s">
-        <v>17</v>
+      <c r="D159" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E159" s="5" t="s">
         <v>0</v>
@@ -5114,8 +5127,8 @@
       <c r="C160" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D160" s="2" t="s">
-        <v>17</v>
+      <c r="D160" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E160" s="5" t="s">
         <v>1</v>
@@ -5218,8 +5231,8 @@
       <c r="C164" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D164" s="2" t="s">
-        <v>17</v>
+      <c r="D164" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E164" s="5" t="s">
         <v>0</v>
@@ -5244,8 +5257,8 @@
       <c r="C165" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D165" s="2" t="s">
-        <v>17</v>
+      <c r="D165" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E165" s="5" t="s">
         <v>1</v>
@@ -5348,8 +5361,8 @@
       <c r="C169" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D169" s="2" t="s">
-        <v>17</v>
+      <c r="D169" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E169" s="5" t="s">
         <v>0</v>
@@ -5374,8 +5387,8 @@
       <c r="C170" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D170" s="2" t="s">
-        <v>17</v>
+      <c r="D170" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E170" s="5" t="s">
         <v>1</v>
@@ -5478,8 +5491,8 @@
       <c r="C174" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D174" s="2" t="s">
-        <v>17</v>
+      <c r="D174" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E174" s="5" t="s">
         <v>0</v>
@@ -5504,8 +5517,8 @@
       <c r="C175" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D175" s="2" t="s">
-        <v>17</v>
+      <c r="D175" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E175" s="5" t="s">
         <v>1</v>
@@ -5608,8 +5621,8 @@
       <c r="C179" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D179" s="2" t="s">
-        <v>17</v>
+      <c r="D179" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E179" s="5" t="s">
         <v>0</v>
@@ -5634,8 +5647,8 @@
       <c r="C180" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D180" s="2" t="s">
-        <v>17</v>
+      <c r="D180" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E180" s="5" t="s">
         <v>1</v>
@@ -5738,8 +5751,8 @@
       <c r="C184" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D184" s="2" t="s">
-        <v>17</v>
+      <c r="D184" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E184" s="5" t="s">
         <v>0</v>
@@ -5764,8 +5777,8 @@
       <c r="C185" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D185" s="2" t="s">
-        <v>17</v>
+      <c r="D185" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E185" s="5" t="s">
         <v>1</v>
@@ -5832,7 +5845,7 @@
         <v>1085036</v>
       </c>
       <c r="I187" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="188" spans="1:9">
@@ -5871,8 +5884,8 @@
       <c r="C189" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D189" s="2" t="s">
-        <v>17</v>
+      <c r="D189" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E189" s="5" t="s">
         <v>0</v>
@@ -5897,8 +5910,8 @@
       <c r="C190" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D190" s="2" t="s">
-        <v>17</v>
+      <c r="D190" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E190" s="5" t="s">
         <v>1</v>
@@ -6001,8 +6014,8 @@
       <c r="C194" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D194" s="2" t="s">
-        <v>17</v>
+      <c r="D194" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E194" s="5" t="s">
         <v>0</v>
@@ -6027,8 +6040,8 @@
       <c r="C195" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D195" s="2" t="s">
-        <v>17</v>
+      <c r="D195" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E195" s="5" t="s">
         <v>1</v>
@@ -6131,8 +6144,8 @@
       <c r="C199" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D199" s="2" t="s">
-        <v>17</v>
+      <c r="D199" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E199" s="5" t="s">
         <v>0</v>
@@ -6157,8 +6170,8 @@
       <c r="C200" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D200" s="2" t="s">
-        <v>17</v>
+      <c r="D200" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E200" s="5" t="s">
         <v>1</v>
@@ -6261,8 +6274,8 @@
       <c r="C204" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D204" s="2" t="s">
-        <v>17</v>
+      <c r="D204" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E204" s="5" t="s">
         <v>0</v>
@@ -6287,8 +6300,8 @@
       <c r="C205" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D205" s="2" t="s">
-        <v>17</v>
+      <c r="D205" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E205" s="5" t="s">
         <v>1</v>
@@ -6391,8 +6404,8 @@
       <c r="C209" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D209" s="2" t="s">
-        <v>17</v>
+      <c r="D209" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E209" s="5" t="s">
         <v>0</v>
@@ -6417,8 +6430,8 @@
       <c r="C210" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D210" s="2" t="s">
-        <v>17</v>
+      <c r="D210" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E210" s="5" t="s">
         <v>1</v>
@@ -6521,8 +6534,8 @@
       <c r="C214" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D214" s="2" t="s">
-        <v>17</v>
+      <c r="D214" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E214" s="5" t="s">
         <v>0</v>
@@ -6547,8 +6560,8 @@
       <c r="C215" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D215" s="2" t="s">
-        <v>17</v>
+      <c r="D215" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E215" s="5" t="s">
         <v>1</v>
@@ -6651,8 +6664,8 @@
       <c r="C219" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D219" s="2" t="s">
-        <v>17</v>
+      <c r="D219" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E219" s="5" t="s">
         <v>0</v>
@@ -6677,8 +6690,8 @@
       <c r="C220" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D220" s="2" t="s">
-        <v>17</v>
+      <c r="D220" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E220" s="5" t="s">
         <v>1</v>
@@ -6781,8 +6794,8 @@
       <c r="C224" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D224" s="2" t="s">
-        <v>17</v>
+      <c r="D224" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E224" s="5" t="s">
         <v>0</v>
@@ -6807,8 +6820,8 @@
       <c r="C225" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D225" s="2" t="s">
-        <v>17</v>
+      <c r="D225" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E225" s="5" t="s">
         <v>1</v>
@@ -6911,8 +6924,8 @@
       <c r="C229" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D229" s="2" t="s">
-        <v>17</v>
+      <c r="D229" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E229" s="5" t="s">
         <v>0</v>
@@ -6937,8 +6950,8 @@
       <c r="C230" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D230" s="2" t="s">
-        <v>17</v>
+      <c r="D230" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E230" s="5" t="s">
         <v>1</v>
@@ -7041,8 +7054,8 @@
       <c r="C234" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D234" s="2" t="s">
-        <v>17</v>
+      <c r="D234" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E234" s="5" t="s">
         <v>0</v>
@@ -7067,8 +7080,8 @@
       <c r="C235" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D235" s="2" t="s">
-        <v>17</v>
+      <c r="D235" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E235" s="5" t="s">
         <v>1</v>
@@ -7171,8 +7184,8 @@
       <c r="C239" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D239" s="2" t="s">
-        <v>17</v>
+      <c r="D239" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E239" s="5" t="s">
         <v>0</v>
@@ -7275,8 +7288,8 @@
       <c r="C243" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D243" s="2" t="s">
-        <v>17</v>
+      <c r="D243" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E243" s="5" t="s">
         <v>1</v>
@@ -7301,8 +7314,8 @@
       <c r="C244" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D244" s="2" t="s">
-        <v>17</v>
+      <c r="D244" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E244" s="5" t="s">
         <v>0</v>
@@ -7327,8 +7340,8 @@
       <c r="C245" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D245" s="2" t="s">
-        <v>17</v>
+      <c r="D245" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E245" s="5" t="s">
         <v>1</v>
@@ -7431,8 +7444,8 @@
       <c r="C249" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D249" s="2" t="s">
-        <v>17</v>
+      <c r="D249" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E249" s="5" t="s">
         <v>0</v>
@@ -7457,8 +7470,8 @@
       <c r="C250" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D250" s="2" t="s">
-        <v>17</v>
+      <c r="D250" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E250" s="5" t="s">
         <v>1</v>
@@ -7499,7 +7512,7 @@
         <v>0</v>
       </c>
       <c r="I251" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="252" spans="1:9">
@@ -7564,8 +7577,8 @@
       <c r="C254" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D254" s="2" t="s">
-        <v>17</v>
+      <c r="D254" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E254" s="5" t="s">
         <v>0</v>
@@ -7590,8 +7603,8 @@
       <c r="C255" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D255" s="2" t="s">
-        <v>17</v>
+      <c r="D255" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E255" s="5" t="s">
         <v>1</v>
@@ -7684,7 +7697,7 @@
         <v>0</v>
       </c>
       <c r="I258" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="259" spans="1:9">
@@ -7697,8 +7710,8 @@
       <c r="C259" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D259" s="2" t="s">
-        <v>17</v>
+      <c r="D259" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E259" s="5" t="s">
         <v>0</v>
@@ -7723,8 +7736,8 @@
       <c r="C260" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D260" s="2" t="s">
-        <v>17</v>
+      <c r="D260" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E260" s="5" t="s">
         <v>1</v>
@@ -7817,7 +7830,7 @@
         <v>0</v>
       </c>
       <c r="I263" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="264" spans="1:9">
@@ -7830,8 +7843,8 @@
       <c r="C264" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D264" s="2" t="s">
-        <v>17</v>
+      <c r="D264" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E264" s="5" t="s">
         <v>0</v>
@@ -7856,8 +7869,8 @@
       <c r="C265" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D265" s="2" t="s">
-        <v>17</v>
+      <c r="D265" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E265" s="5" t="s">
         <v>1</v>
@@ -7960,8 +7973,8 @@
       <c r="C269" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D269" s="2" t="s">
-        <v>17</v>
+      <c r="D269" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E269" s="5" t="s">
         <v>0</v>
@@ -7986,8 +7999,8 @@
       <c r="C270" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D270" s="2" t="s">
-        <v>17</v>
+      <c r="D270" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E270" s="5" t="s">
         <v>1</v>
@@ -8090,8 +8103,8 @@
       <c r="C274" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D274" s="2" t="s">
-        <v>17</v>
+      <c r="D274" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E274" s="5" t="s">
         <v>0</v>
@@ -8116,8 +8129,8 @@
       <c r="C275" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D275" s="2" t="s">
-        <v>17</v>
+      <c r="D275" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E275" s="5" t="s">
         <v>1</v>
@@ -8220,8 +8233,8 @@
       <c r="C279" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D279" s="2" t="s">
-        <v>17</v>
+      <c r="D279" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E279" s="5" t="s">
         <v>0</v>
@@ -8246,8 +8259,8 @@
       <c r="C280" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D280" s="2" t="s">
-        <v>17</v>
+      <c r="D280" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E280" s="5" t="s">
         <v>1</v>
@@ -8350,8 +8363,8 @@
       <c r="C284" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D284" s="2" t="s">
-        <v>17</v>
+      <c r="D284" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E284" s="5" t="s">
         <v>0</v>
@@ -8376,8 +8389,8 @@
       <c r="C285" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D285" s="2" t="s">
-        <v>17</v>
+      <c r="D285" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E285" s="5" t="s">
         <v>1</v>
@@ -8480,8 +8493,8 @@
       <c r="C289" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D289" s="2" t="s">
-        <v>17</v>
+      <c r="D289" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E289" s="5" t="s">
         <v>0</v>
@@ -8506,8 +8519,8 @@
       <c r="C290" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D290" s="2" t="s">
-        <v>17</v>
+      <c r="D290" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E290" s="5" t="s">
         <v>1</v>
@@ -8610,8 +8623,8 @@
       <c r="C294" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D294" s="2" t="s">
-        <v>17</v>
+      <c r="D294" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E294" s="5" t="s">
         <v>0</v>
@@ -8636,8 +8649,8 @@
       <c r="C295" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D295" s="2" t="s">
-        <v>17</v>
+      <c r="D295" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E295" s="5" t="s">
         <v>1</v>
@@ -8740,8 +8753,8 @@
       <c r="C299" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D299" s="2" t="s">
-        <v>17</v>
+      <c r="D299" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E299" s="5" t="s">
         <v>0</v>
@@ -8766,8 +8779,8 @@
       <c r="C300" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D300" s="2" t="s">
-        <v>17</v>
+      <c r="D300" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E300" s="5" t="s">
         <v>1</v>
@@ -8870,8 +8883,8 @@
       <c r="C304" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D304" s="2" t="s">
-        <v>17</v>
+      <c r="D304" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E304" s="5" t="s">
         <v>0</v>
@@ -8896,8 +8909,8 @@
       <c r="C305" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D305" s="2" t="s">
-        <v>17</v>
+      <c r="D305" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E305" s="5" t="s">
         <v>1</v>
@@ -9000,8 +9013,8 @@
       <c r="C309" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D309" s="2" t="s">
-        <v>17</v>
+      <c r="D309" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E309" s="5" t="s">
         <v>0</v>
@@ -9026,8 +9039,8 @@
       <c r="C310" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D310" s="2" t="s">
-        <v>17</v>
+      <c r="D310" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E310" s="5" t="s">
         <v>1</v>
@@ -9052,8 +9065,8 @@
       <c r="C311" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D311" s="2" t="s">
-        <v>17</v>
+      <c r="D311" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E311" s="5" t="s">
         <v>0</v>
@@ -9156,8 +9169,8 @@
       <c r="C315" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D315" s="2" t="s">
-        <v>17</v>
+      <c r="D315" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E315" s="5" t="s">
         <v>1</v>
@@ -9182,8 +9195,8 @@
       <c r="C316" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D316" s="2" t="s">
-        <v>17</v>
+      <c r="D316" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E316" s="5" t="s">
         <v>0</v>
@@ -9224,7 +9237,7 @@
         <v>1194671</v>
       </c>
       <c r="I317" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="318" spans="1:9">
@@ -9289,8 +9302,8 @@
       <c r="C320" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D320" s="2" t="s">
-        <v>17</v>
+      <c r="D320" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E320" s="5" t="s">
         <v>1</v>
@@ -9315,8 +9328,8 @@
       <c r="C321" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D321" s="2" t="s">
-        <v>17</v>
+      <c r="D321" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E321" s="5" t="s">
         <v>0</v>
@@ -9357,7 +9370,7 @@
         <v>1194671</v>
       </c>
       <c r="I322" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="323" spans="1:9">
@@ -9417,32 +9430,84 @@
         <v>45810</v>
       </c>
       <c r="B325" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C325" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C325" s="9" t="s">
+      <c r="D325" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D325" s="9" t="s">
+      <c r="E325" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F325" s="7">
+        <v>1</v>
+      </c>
+      <c r="G325" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H325" s="7">
+        <v>1</v>
+      </c>
+      <c r="I325" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E325" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F325" s="7">
-        <v>1</v>
-      </c>
-      <c r="G325" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H325" s="7">
-        <v>1</v>
-      </c>
-      <c r="I325" s="9" t="s">
-        <v>33</v>
+    </row>
+    <row r="326" spans="1:9" ht="18">
+      <c r="A326" s="3">
+        <v>45810</v>
+      </c>
+      <c r="B326" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D326" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E326" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F326" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="G326" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H326" s="5">
+        <v>7897.04</v>
+      </c>
+    </row>
+    <row r="327" spans="1:9" ht="18">
+      <c r="A327" s="3">
+        <v>45810</v>
+      </c>
+      <c r="B327" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C327" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D327" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E327" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F327" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="G327" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H327" s="5">
+        <v>7897.04</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I319" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I325" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>